<commit_message>
working on the complementarity
</commit_message>
<xml_diff>
--- a/Generation Data.xlsx
+++ b/Generation Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta\Desktop\Sustainable Energy\OMPS\Project\optimization_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8766D4-F838-4742-AD13-77ECA5DBF3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7823174-781F-47EB-AFAE-2BCF9AD9F891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="2835" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generation_investor" sheetId="1" r:id="rId1"/>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,24 +475,12 @@
         <v>15</v>
       </c>
       <c r="C6" s="1">
-        <v>60</v>
+        <f>60+155</f>
+        <v>215</v>
       </c>
       <c r="D6" s="1">
-        <v>26.11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1">
-        <v>155</v>
-      </c>
-      <c r="D7" s="1">
-        <v>10.52</v>
+        <f>(26.11+10.52)/2</f>
+        <v>18.314999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -502,10 +490,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AC9C34-CEA6-40FB-88E5-8DD177C1D408}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,24 +576,12 @@
         <v>23</v>
       </c>
       <c r="C6" s="1">
-        <v>310</v>
+        <f>350+310</f>
+        <v>660</v>
       </c>
       <c r="D6" s="1">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1">
-        <v>350</v>
-      </c>
-      <c r="D7" s="1">
-        <v>10.89</v>
+        <f>(10.52+10.89)/2</f>
+        <v>10.705</v>
       </c>
     </row>
   </sheetData>
@@ -620,6 +596,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AEDD2C58C424B74499DE9AAA38D1F837" ma:contentTypeVersion="4" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="702f087d0813d5dfa38d019e1cfe3dbe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="59a1f2c9-9aa0-4700-bb29-973d29195b9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f1c68433e2c2319791049a96af9fb53" ns2:_="">
     <xsd:import namespace="59a1f2c9-9aa0-4700-bb29-973d29195b9e"/>
@@ -763,15 +748,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36AF9D7E-4190-47C9-A25E-E341BDEC68ED}">
   <ds:schemaRefs>
@@ -782,6 +758,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16E2F5C7-B52B-483C-B6AD-926B66F164B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BCEB3E-2236-4D28-844D-4CC52B255655}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -797,12 +781,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16E2F5C7-B52B-483C-B6AD-926B66F164B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
debugging. all indexes to 0, all variables created for all nodes
</commit_message>
<xml_diff>
--- a/Generation Data.xlsx
+++ b/Generation Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta\Desktop\Sustainable Energy\OMPS\Project\optimization_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7823174-781F-47EB-AFAE-2BCF9AD9F891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDF5279-AC77-4343-8A55-4825CCB5C042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generation_investor" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -95,13 +95,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,46 +453,320 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>7</v>
-      </c>
       <c r="C4" s="1">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>20.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>13</v>
-      </c>
       <c r="C5" s="1">
-        <v>591</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>20.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>350</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1">
+        <v>591</v>
+      </c>
+      <c r="D14" s="1">
+        <v>20.93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1">
         <v>15</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C16" s="1">
         <f>60+155</f>
         <v>215</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D16" s="1">
         <f>(26.11+10.52)/2</f>
         <v>18.314999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <f>B16+1</f>
+        <v>16</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ref="B18:B24" si="0">B17+1</f>
+        <v>17</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <f>B22+1</f>
+        <v>22</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -490,10 +776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AC9C34-CEA6-40FB-88E5-8DD177C1D408}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,55 +800,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>10.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>18</v>
+        <f>B2+1</f>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>6.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>21</v>
+        <f t="shared" ref="B4:B16" si="0">B3+1</f>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>5.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1">
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -570,18 +859,295 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1">
+        <v>155</v>
+      </c>
+      <c r="D17" s="1">
+        <v>10.52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1">
+        <v>400</v>
+      </c>
+      <c r="D19" s="1">
+        <v>6.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1">
+        <v>400</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5.47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1">
+        <v>300</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1">
         <v>23</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C24" s="1">
         <f>350+310</f>
         <v>660</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D24" s="1">
         <f>(10.52+10.89)/2</f>
         <v>10.705</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>